<commit_message>
From latest fitting, probably hopefully going to run with these data & results
</commit_message>
<xml_diff>
--- a/data/fromR/bottom_ten_threatened.xlsx
+++ b/data/fromR/bottom_ten_threatened.xlsx
@@ -1,39 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/Rstudio_Git/threatRF/data/fromR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C81AE0EA-725C-3644-8B40-F697200BAE96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{983F30A2-14AD-0D4E-8CF4-B2A667337FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1820" windowWidth="27240" windowHeight="16440"/>
+    <workbookView xWindow="47320" yWindow="12080" windowWidth="28040" windowHeight="17440" xr2:uid="{8E3FC835-3CA1-B040-A0A3-94B502A2F72B}"/>
   </bookViews>
   <sheets>
     <sheet name="bottom_ten_threatened" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="102">
   <si>
     <t>taxon</t>
   </si>
@@ -44,7 +31,130 @@
     <t>species</t>
   </si>
   <si>
-    <t>lepidoptera</t>
+    <t>threat_rank</t>
+  </si>
+  <si>
+    <t>perc_votes_threatened</t>
+  </si>
+  <si>
+    <t>lepidopterans</t>
+  </si>
+  <si>
+    <t>Antheraea</t>
+  </si>
+  <si>
+    <t>polyphemus</t>
+  </si>
+  <si>
+    <t>Hemaris</t>
+  </si>
+  <si>
+    <t>diffinis</t>
+  </si>
+  <si>
+    <t>Hypsopygia</t>
+  </si>
+  <si>
+    <t>olinalis</t>
+  </si>
+  <si>
+    <t>Alypia</t>
+  </si>
+  <si>
+    <t>octomaculata</t>
+  </si>
+  <si>
+    <t>Crambus</t>
+  </si>
+  <si>
+    <t>agitatellus</t>
+  </si>
+  <si>
+    <t>Cycnia</t>
+  </si>
+  <si>
+    <t>tenera</t>
+  </si>
+  <si>
+    <t>Helicoverpa</t>
+  </si>
+  <si>
+    <t>zea</t>
+  </si>
+  <si>
+    <t>Marimatha</t>
+  </si>
+  <si>
+    <t>nigrofimbria</t>
+  </si>
+  <si>
+    <t>Nomophila</t>
+  </si>
+  <si>
+    <t>nearctica</t>
+  </si>
+  <si>
+    <t>Palthis</t>
+  </si>
+  <si>
+    <t>asopialis</t>
+  </si>
+  <si>
+    <t>Argyria</t>
+  </si>
+  <si>
+    <t>nivalis</t>
+  </si>
+  <si>
+    <t>Callima</t>
+  </si>
+  <si>
+    <t>argenticinctella</t>
+  </si>
+  <si>
+    <t>Costaconvexa</t>
+  </si>
+  <si>
+    <t>centrostrigaria</t>
+  </si>
+  <si>
+    <t>Eacles</t>
+  </si>
+  <si>
+    <t>imperialis</t>
+  </si>
+  <si>
+    <t>Epimecis</t>
+  </si>
+  <si>
+    <t>hortaria</t>
+  </si>
+  <si>
+    <t>Euchaetes</t>
+  </si>
+  <si>
+    <t>egle</t>
+  </si>
+  <si>
+    <t>Eumorpha</t>
+  </si>
+  <si>
+    <t>pandorus</t>
+  </si>
+  <si>
+    <t>Harrisina</t>
+  </si>
+  <si>
+    <t>americana</t>
+  </si>
+  <si>
+    <t>thysbe</t>
+  </si>
+  <si>
+    <t>Hylephila</t>
+  </si>
+  <si>
+    <t>phyleus</t>
   </si>
   <si>
     <t>Hyphantria</t>
@@ -53,100 +163,19 @@
     <t>cunea</t>
   </si>
   <si>
-    <t>Marimatha</t>
-  </si>
-  <si>
-    <t>nigrofimbria</t>
-  </si>
-  <si>
-    <t>Nomophila</t>
-  </si>
-  <si>
-    <t>nearctica</t>
-  </si>
-  <si>
-    <t>Palthis</t>
-  </si>
-  <si>
-    <t>asopialis</t>
-  </si>
-  <si>
-    <t>Hemaris</t>
-  </si>
-  <si>
-    <t>diffinis</t>
-  </si>
-  <si>
-    <t>Atteva</t>
-  </si>
-  <si>
-    <t>punctella</t>
-  </si>
-  <si>
-    <t>Hylephila</t>
-  </si>
-  <si>
-    <t>phyleus</t>
-  </si>
-  <si>
     <t>Malacosoma</t>
   </si>
   <si>
-    <t>americana</t>
-  </si>
-  <si>
-    <t>Pyrrharctia</t>
-  </si>
-  <si>
-    <t>isabella</t>
-  </si>
-  <si>
-    <t>Actias</t>
-  </si>
-  <si>
-    <t>luna</t>
-  </si>
-  <si>
-    <t>Cycnia</t>
-  </si>
-  <si>
-    <t>tenera</t>
-  </si>
-  <si>
-    <t>Agrotis</t>
-  </si>
-  <si>
-    <t>ipsilon</t>
-  </si>
-  <si>
-    <t>Choristoneura</t>
-  </si>
-  <si>
-    <t>rosaceana</t>
-  </si>
-  <si>
-    <t>Cisseps</t>
-  </si>
-  <si>
-    <t>fulvicollis</t>
-  </si>
-  <si>
-    <t>Euptoieta</t>
-  </si>
-  <si>
-    <t>claudia</t>
-  </si>
-  <si>
-    <t>Orthonama</t>
-  </si>
-  <si>
-    <t>obstipata</t>
-  </si>
-  <si>
-    <t>Parallelia</t>
-  </si>
-  <si>
-    <t>bistriaris</t>
+    <t>Papilio</t>
+  </si>
+  <si>
+    <t>troilus</t>
+  </si>
+  <si>
+    <t>Pleuroprucha</t>
+  </si>
+  <si>
+    <t>insulsaria</t>
   </si>
   <si>
     <t>Schinia</t>
@@ -161,13 +190,40 @@
     <t>cardui</t>
   </si>
   <si>
-    <t>plantae</t>
-  </si>
-  <si>
-    <t>Elymus</t>
-  </si>
-  <si>
-    <t>virginicus</t>
+    <t>virginiensis</t>
+  </si>
+  <si>
+    <t>Zale</t>
+  </si>
+  <si>
+    <t>lunata</t>
+  </si>
+  <si>
+    <t>plants</t>
+  </si>
+  <si>
+    <t>Carex</t>
+  </si>
+  <si>
+    <t>comosa</t>
+  </si>
+  <si>
+    <t>Andropogon</t>
+  </si>
+  <si>
+    <t>glomeratus</t>
+  </si>
+  <si>
+    <t>annectens</t>
+  </si>
+  <si>
+    <t>Dichanthelium</t>
+  </si>
+  <si>
+    <t>scoparium</t>
+  </si>
+  <si>
+    <t>longii</t>
   </si>
   <si>
     <t>Juncus</t>
@@ -176,10 +232,73 @@
     <t>dichotomus</t>
   </si>
   <si>
-    <t>Carex</t>
-  </si>
-  <si>
-    <t>longii</t>
+    <t>Coleataenia</t>
+  </si>
+  <si>
+    <t>anceps</t>
+  </si>
+  <si>
+    <t>Hydrocotyle</t>
+  </si>
+  <si>
+    <t>umbellata</t>
+  </si>
+  <si>
+    <t>Packera</t>
+  </si>
+  <si>
+    <t>dubia</t>
+  </si>
+  <si>
+    <t>Polygala</t>
+  </si>
+  <si>
+    <t>mariana</t>
+  </si>
+  <si>
+    <t>Eupatorium</t>
+  </si>
+  <si>
+    <t>album</t>
+  </si>
+  <si>
+    <t>Polypremum</t>
+  </si>
+  <si>
+    <t>procumbens</t>
+  </si>
+  <si>
+    <t>lupulina</t>
+  </si>
+  <si>
+    <t>rotundifolium</t>
+  </si>
+  <si>
+    <t>Fimbristylis</t>
+  </si>
+  <si>
+    <t>autumnalis</t>
+  </si>
+  <si>
+    <t>Vicia</t>
+  </si>
+  <si>
+    <t>lathyroides</t>
+  </si>
+  <si>
+    <t>Amelanchier</t>
+  </si>
+  <si>
+    <t>obovalis</t>
+  </si>
+  <si>
+    <t>crinita</t>
+  </si>
+  <si>
+    <t>Phoradendron</t>
+  </si>
+  <si>
+    <t>leucarpum</t>
   </si>
   <si>
     <t>Cyperus</t>
@@ -188,192 +307,50 @@
     <t>retrorsus</t>
   </si>
   <si>
-    <t>Polygala</t>
-  </si>
-  <si>
-    <t>mariana</t>
-  </si>
-  <si>
-    <t>Eupatorium</t>
-  </si>
-  <si>
-    <t>album</t>
-  </si>
-  <si>
-    <t>Lobelia</t>
-  </si>
-  <si>
-    <t>puberula</t>
-  </si>
-  <si>
-    <t>Panicum</t>
-  </si>
-  <si>
-    <t>virgatum</t>
-  </si>
-  <si>
-    <t>Fimbristylis</t>
-  </si>
-  <si>
-    <t>autumnalis</t>
-  </si>
-  <si>
-    <t>Dichanthelium</t>
-  </si>
-  <si>
-    <t>scoparium</t>
-  </si>
-  <si>
-    <t>vulpinoidea</t>
-  </si>
-  <si>
-    <t>comosa</t>
-  </si>
-  <si>
-    <t>Gaylussacia</t>
-  </si>
-  <si>
-    <t>frondosa</t>
-  </si>
-  <si>
-    <t>lupulina</t>
-  </si>
-  <si>
-    <t>threat rank</t>
-  </si>
-  <si>
-    <t>vote fraction (threatened)</t>
-  </si>
-  <si>
-    <t>Status elsewhere?</t>
-  </si>
-  <si>
-    <t>Northern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Appalachian </t>
+    <t>status elsewhere</t>
+  </si>
+  <si>
+    <t>northern</t>
+  </si>
+  <si>
+    <t>appalachian</t>
   </si>
   <si>
     <t>notes</t>
   </si>
   <si>
-    <t>S5 ON; ID, PA</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>2-17 RTE list notes that NY is at Northern Range limit (not obvious from iNaturalist records, e.g. good-looking record in VT from 2022). https://guides.nynhp.org/black-bordered-lemon-moth/</t>
-  </si>
-  <si>
-    <t>S1 NY, S4 PA</t>
-  </si>
-  <si>
-    <t>S5 PA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N </t>
-  </si>
-  <si>
-    <t>S4 NY, S3 ON</t>
-  </si>
-  <si>
-    <t>S4 ON, S5 PA</t>
-  </si>
-  <si>
-    <t>S4 ON, S5 PA, KY</t>
-  </si>
-  <si>
-    <t>S5 Everywhere, including MD</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Synonym </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Papilio phyleus</t>
-    </r>
-  </si>
-  <si>
-    <t>S5 ON, PA</t>
-  </si>
-  <si>
-    <t>S4 ID, S5 ON, PA</t>
-  </si>
-  <si>
-    <t>S4 QE, S5 ON, PA, VT</t>
-  </si>
-  <si>
-    <t>S4 WV, S5 ON, NC, IL, IN, KY</t>
-  </si>
-  <si>
-    <t>S1 PA, WV, OH; S2 NY, S4 DE, GA, S5 NC, VA, NJ</t>
-  </si>
-  <si>
-    <t>More southern range, temporary wetland specialist</t>
-  </si>
-  <si>
-    <t>S1 OH, WV, S2 KY, PA; S3 NY; S4 NJ, DE; S5 VA</t>
-  </si>
-  <si>
-    <t>Habitat specialist (wetland margins) and wide variety of statuses across E N America</t>
-  </si>
-  <si>
-    <t>S1 MA, NY; S2 KY; S4 NJ; S5 GA, NC, VA</t>
-  </si>
-  <si>
-    <t>Dry Sandy Soil Specialist, largely Southern sp</t>
-  </si>
-  <si>
-    <t>S1 TN, S2 NJ, S4 DE, NC; S5 KY, VA</t>
-  </si>
-  <si>
-    <t>S1 CT, OH, S3 IN, WV; S4 DE; S5 NC, VA, KY</t>
-  </si>
-  <si>
-    <t>S1 PA; S4 KY; S5 NC, WV, VA</t>
-  </si>
-  <si>
-    <t>S2 QE; S3 VT;  S4 ON, KY; S5 IL, NC, VA, NC</t>
-  </si>
-  <si>
-    <t>S1 VT; S2 ME; S3 IL; S4 NC, ON, QE; S5 KY, VA, WV, NJ, NY</t>
-  </si>
-  <si>
-    <t>SH WV, MA; S1 IL, IN, OH, PA, NY; S4 NJ; S5 NC, VA, DE</t>
+    <t>n</t>
+  </si>
+  <si>
+    <t>S3 VT; S4 NB, NS; S5 PA, IN, ON</t>
+  </si>
+  <si>
+    <t>Possible missed synonym for Urola nivalis, skip this one.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="Aptos Display"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -381,7 +358,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -389,7 +366,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -397,35 +374,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -433,7 +410,7 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -441,14 +418,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -456,14 +433,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -471,7 +448,7 @@
       <i/>
       <sz val="12"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -479,27 +456,19 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -677,6 +646,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -842,9 +817,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -914,39 +887,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -998,7 +971,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1109,13 +1082,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -1124,6 +1090,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1188,67 +1161,84 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8464DB8-FE0D-1C41-97DA-9802D510FE97}">
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="6" max="6" width="46.33203125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>73</v>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1257,24 +1247,24 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="H2" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1282,28 +1272,22 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
-        <v>77</v>
-      </c>
       <c r="G3" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I3" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1311,357 +1295,381 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
-        <v>78</v>
-      </c>
       <c r="G4" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="H4" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>80</v>
+        <v>2E-3</v>
       </c>
       <c r="G5" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="H5" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <v>2E-3</v>
       </c>
-      <c r="F6" t="s">
-        <v>82</v>
-      </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="H6" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E7">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>81</v>
+        <v>2E-3</v>
       </c>
       <c r="G7" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="H7" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E8">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>83</v>
+        <v>2E-3</v>
       </c>
       <c r="G8" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="H8" t="s">
-        <v>75</v>
-      </c>
-      <c r="I8" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>85</v>
+        <v>2E-3</v>
       </c>
       <c r="G9" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="H9" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E10">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="F10" t="s">
-        <v>86</v>
+        <v>2E-3</v>
       </c>
       <c r="G10" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="H10" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="F11" t="s">
-        <v>87</v>
+        <v>2E-3</v>
       </c>
       <c r="G11" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="H11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <v>6.0000000000000001E-3</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13">
-        <v>8.0000000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D14">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14">
-        <v>8.0000000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>99</v>
+      </c>
+      <c r="H14" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D15">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15">
-        <v>8.0000000000000002E-3</v>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D16">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E16">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>99</v>
+      </c>
+      <c r="H16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D17">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D18">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>99</v>
+      </c>
+      <c r="H18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D19">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D20">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E20">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G20" t="s">
+        <v>99</v>
+      </c>
+      <c r="H20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
         <v>43</v>
@@ -1670,24 +1678,21 @@
         <v>44</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E21">
-        <v>0.13400000000000001</v>
-      </c>
-      <c r="F21" t="s">
-        <v>88</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="G21" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="H21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
         <v>45</v>
@@ -1696,275 +1701,251 @@
         <v>46</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E22">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="F22" t="s">
-        <v>89</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="G22" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="H22" t="s">
-        <v>75</v>
-      </c>
-      <c r="I22" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
         <v>47</v>
       </c>
       <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23">
+        <v>11</v>
+      </c>
+      <c r="E23">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G23" t="s">
+        <v>99</v>
+      </c>
+      <c r="H23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" t="s">
         <v>48</v>
       </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="E23">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="F23" t="s">
-        <v>91</v>
-      </c>
-      <c r="G23" t="s">
-        <v>75</v>
-      </c>
-      <c r="H23" t="s">
-        <v>75</v>
-      </c>
-      <c r="I23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>49</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24">
+        <v>11</v>
+      </c>
+      <c r="E24">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>99</v>
+      </c>
+      <c r="H24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" t="s">
         <v>50</v>
       </c>
-      <c r="D24">
-        <v>4</v>
-      </c>
-      <c r="E24">
-        <v>0.15</v>
-      </c>
-      <c r="F24" t="s">
-        <v>93</v>
-      </c>
-      <c r="G24" t="s">
-        <v>75</v>
-      </c>
-      <c r="H24" t="s">
-        <v>75</v>
-      </c>
-      <c r="I24" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>51</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G25" t="s">
+        <v>99</v>
+      </c>
+      <c r="H25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
         <v>52</v>
       </c>
-      <c r="D25">
-        <v>5</v>
-      </c>
-      <c r="E25">
-        <v>0.154</v>
-      </c>
-      <c r="F25" t="s">
-        <v>95</v>
-      </c>
-      <c r="G25" t="s">
-        <v>75</v>
-      </c>
-      <c r="H25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>42</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>53</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26">
+        <v>11</v>
+      </c>
+      <c r="E26">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
         <v>54</v>
       </c>
-      <c r="D26">
-        <v>6</v>
-      </c>
-      <c r="E26">
-        <v>0.16</v>
-      </c>
-      <c r="F26" t="s">
-        <v>96</v>
-      </c>
-      <c r="G26" t="s">
-        <v>75</v>
-      </c>
-      <c r="H26" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>55</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27">
+        <v>11</v>
+      </c>
+      <c r="E27">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G27" t="s">
+        <v>99</v>
+      </c>
+      <c r="H27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="s">
         <v>56</v>
       </c>
-      <c r="D27">
-        <v>7</v>
-      </c>
-      <c r="E27">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="F27" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" t="s">
-        <v>75</v>
-      </c>
-      <c r="H27" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="D28">
+        <v>11</v>
+      </c>
+      <c r="E28">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G28" t="s">
+        <v>99</v>
+      </c>
+      <c r="H28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
         <v>57</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>58</v>
       </c>
-      <c r="D28">
-        <v>7</v>
-      </c>
-      <c r="E28">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="F28" t="s">
-        <v>98</v>
-      </c>
-      <c r="G28" t="s">
-        <v>75</v>
-      </c>
-      <c r="H28" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="D29">
+        <v>11</v>
+      </c>
+      <c r="E29">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G29" t="s">
+        <v>99</v>
+      </c>
+      <c r="H29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>59</v>
       </c>
-      <c r="C29" t="s">
+      <c r="B30" t="s">
         <v>60</v>
       </c>
-      <c r="D29">
-        <v>9</v>
-      </c>
-      <c r="E29">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="F29" t="s">
-        <v>99</v>
-      </c>
-      <c r="G29" t="s">
-        <v>75</v>
-      </c>
-      <c r="H29" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>61</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="G30" t="s">
+        <v>99</v>
+      </c>
+      <c r="H30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" t="s">
         <v>62</v>
-      </c>
-      <c r="D30">
-        <v>10</v>
-      </c>
-      <c r="E30">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="F30" t="s">
-        <v>100</v>
-      </c>
-      <c r="G30" t="s">
-        <v>75</v>
-      </c>
-      <c r="H30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" t="s">
-        <v>47</v>
       </c>
       <c r="C31" t="s">
         <v>63</v>
       </c>
       <c r="D31">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E31">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0.152</v>
+      </c>
+      <c r="G31" t="s">
+        <v>99</v>
+      </c>
+      <c r="H31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
         <v>64</v>
       </c>
       <c r="D32">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E32">
-        <v>0.184</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.16</v>
+      </c>
+      <c r="G32" t="s">
+        <v>99</v>
+      </c>
+      <c r="H32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
         <v>65</v>
@@ -1973,27 +1954,330 @@
         <v>66</v>
       </c>
       <c r="D33">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E33">
-        <v>0.184</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.17</v>
+      </c>
+      <c r="G33" t="s">
+        <v>99</v>
+      </c>
+      <c r="H33" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
         <v>67</v>
       </c>
       <c r="D34">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E34">
-        <v>0.186</v>
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="G34" t="s">
+        <v>99</v>
+      </c>
+      <c r="H34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35">
+        <v>5</v>
+      </c>
+      <c r="E35">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="G35" t="s">
+        <v>99</v>
+      </c>
+      <c r="H35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36">
+        <v>7</v>
+      </c>
+      <c r="E36">
+        <v>0.182</v>
+      </c>
+      <c r="G36" t="s">
+        <v>99</v>
+      </c>
+      <c r="H36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37">
+        <v>8</v>
+      </c>
+      <c r="E37">
+        <v>0.188</v>
+      </c>
+      <c r="G37" t="s">
+        <v>99</v>
+      </c>
+      <c r="H37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38">
+        <v>9</v>
+      </c>
+      <c r="E38">
+        <v>0.192</v>
+      </c>
+      <c r="G38" t="s">
+        <v>99</v>
+      </c>
+      <c r="H38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39">
+        <v>9</v>
+      </c>
+      <c r="E39">
+        <v>0.192</v>
+      </c>
+      <c r="G39" t="s">
+        <v>99</v>
+      </c>
+      <c r="H39" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40">
+        <v>11</v>
+      </c>
+      <c r="E40">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="G40" t="s">
+        <v>99</v>
+      </c>
+      <c r="H40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41">
+        <v>11</v>
+      </c>
+      <c r="E41">
+        <v>0.19400000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42">
+        <v>13</v>
+      </c>
+      <c r="E42">
+        <v>0.19600000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" t="s">
+        <v>83</v>
+      </c>
+      <c r="D43">
+        <v>13</v>
+      </c>
+      <c r="E43">
+        <v>0.19600000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44">
+        <v>13</v>
+      </c>
+      <c r="E44">
+        <v>0.19600000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" t="s">
+        <v>87</v>
+      </c>
+      <c r="D45">
+        <v>16</v>
+      </c>
+      <c r="E45">
+        <v>0.20200000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" t="s">
+        <v>88</v>
+      </c>
+      <c r="C46" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46">
+        <v>17</v>
+      </c>
+      <c r="E46">
+        <v>0.20399999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47">
+        <v>17</v>
+      </c>
+      <c r="E47">
+        <v>0.20399999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48">
+        <v>17</v>
+      </c>
+      <c r="E48">
+        <v>0.20399999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49">
+        <v>20</v>
+      </c>
+      <c r="E49">
+        <v>0.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>